<commit_message>
refactor: DMS sheet view sheet
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-analytics-olav.xlsx
+++ b/docs/artifacts/rules/dms-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6BC618-21DA-472E-97C9-2B1A983B0D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2870D5-A4B0-4065-9559-11A7013FCC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="190">
   <si>
     <t>role</t>
   </si>
@@ -591,6 +591,12 @@
   </si>
   <si>
     <t>power:EnergyArea</t>
+  </si>
+  <si>
+    <t>power:Polygon</t>
+  </si>
+  <si>
+    <t>power:Point</t>
   </si>
 </sst>
 </file>
@@ -989,7 +995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1101,9 +1107,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2519,18 +2525,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:G10"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="7" width="13" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
@@ -2569,10 +2577,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" t="s">
+        <v>189</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -2580,13 +2594,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>188</v>
+      </c>
+      <c r="F4" t="s">
+        <v>188</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -2594,13 +2611,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -2608,10 +2622,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -2619,10 +2633,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -2630,23 +2644,12 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="G8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2664,7 +2667,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
refactor: addded indexes in DMS sheet
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-analytics-olav.xlsx
+++ b/docs/artifacts/rules/dms-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2870D5-A4B0-4065-9559-11A7013FCC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB92744-FF76-4960-ABCC-C5EA03573A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="194">
   <si>
     <t>role</t>
   </si>
@@ -597,6 +597,18 @@
   </si>
   <si>
     <t>power:Point</t>
+  </si>
+  <si>
+    <t>name_index</t>
+  </si>
+  <si>
+    <t>algorithm_index</t>
+  </si>
+  <si>
+    <t>type_index</t>
+  </si>
+  <si>
+    <t>source_index</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1107,9 +1119,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,7 +1136,8 @@
     <col min="12" max="12" width="21.44140625" customWidth="1"/>
     <col min="13" max="13" width="14.44140625" customWidth="1"/>
     <col min="14" max="14" width="21.44140625" customWidth="1"/>
-    <col min="15" max="16" width="13" customWidth="1"/>
+    <col min="15" max="15" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
@@ -1988,7 +2001,9 @@
       <c r="N25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O25" s="4"/>
+      <c r="O25" s="4" t="s">
+        <v>190</v>
+      </c>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
@@ -2024,7 +2039,9 @@
       <c r="N26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="O26" s="4"/>
+      <c r="O26" s="4" t="s">
+        <v>192</v>
+      </c>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
@@ -2060,7 +2077,9 @@
       <c r="N27" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="O27" s="4"/>
+      <c r="O27" s="4" t="s">
+        <v>193</v>
+      </c>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
@@ -2090,13 +2109,13 @@
         <v>71</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>71</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
@@ -2368,7 +2387,9 @@
       <c r="N36" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O36" s="5"/>
+      <c r="O36" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="P36" s="5"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
@@ -2404,7 +2425,9 @@
       <c r="N37" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="O37" s="5"/>
+      <c r="O37" s="5" t="s">
+        <v>191</v>
+      </c>
       <c r="P37" s="5"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[NEAT-160] Deploy Olav DMS model (#375)
* refactor: first draft DMS sheets

* docs: Olav DMS as expected

* tests: added failing test for conversion

* feat: Convert to correct container

* refactor: DMS sheet view sheet

* tests: extended test

* feat; set view implements

* refactor: remove debug code

* tests: added failing test

* feat: convert view to reference

* feat: Reference container

* tests: Added export Olav test

* refactor: addded indexes in DMS sheet

* tests: Added integration test for deployment

* docs; Fix some typos

* docs; finish deploy section
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-analytics-olav.xlsx
+++ b/docs/artifacts/rules/dms-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2870D5-A4B0-4065-9559-11A7013FCC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB92744-FF76-4960-ABCC-C5EA03573A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="194">
   <si>
     <t>role</t>
   </si>
@@ -597,6 +597,18 @@
   </si>
   <si>
     <t>power:Point</t>
+  </si>
+  <si>
+    <t>name_index</t>
+  </si>
+  <si>
+    <t>algorithm_index</t>
+  </si>
+  <si>
+    <t>type_index</t>
+  </si>
+  <si>
+    <t>source_index</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1107,9 +1119,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,7 +1136,8 @@
     <col min="12" max="12" width="21.44140625" customWidth="1"/>
     <col min="13" max="13" width="14.44140625" customWidth="1"/>
     <col min="14" max="14" width="21.44140625" customWidth="1"/>
-    <col min="15" max="16" width="13" customWidth="1"/>
+    <col min="15" max="15" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
@@ -1988,7 +2001,9 @@
       <c r="N25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O25" s="4"/>
+      <c r="O25" s="4" t="s">
+        <v>190</v>
+      </c>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
@@ -2024,7 +2039,9 @@
       <c r="N26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="O26" s="4"/>
+      <c r="O26" s="4" t="s">
+        <v>192</v>
+      </c>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
@@ -2060,7 +2077,9 @@
       <c r="N27" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="O27" s="4"/>
+      <c r="O27" s="4" t="s">
+        <v>193</v>
+      </c>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
@@ -2090,13 +2109,13 @@
         <v>71</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>71</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
@@ -2368,7 +2387,9 @@
       <c r="N36" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O36" s="5"/>
+      <c r="O36" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="P36" s="5"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
@@ -2404,7 +2425,9 @@
       <c r="N37" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="O37" s="5"/>
+      <c r="O37" s="5" t="s">
+        <v>191</v>
+      </c>
       <c r="P37" s="5"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
refactor: update ref rules
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-analytics-olav.xlsx
+++ b/docs/artifacts/rules/dms-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB62836-FD62-429D-8907-538417BA4EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D33C57-3DE0-48D7-B7F1-45DA8EF94421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="197">
   <si>
     <t>role</t>
   </si>
@@ -204,9 +204,6 @@
   </si>
   <si>
     <t>powerForecasts</t>
-  </si>
-  <si>
-    <t>multiedge</t>
   </si>
   <si>
     <t>PowerForecast</t>
@@ -1039,10 +1036,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1139,7 +1136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
@@ -1254,7 +1251,7 @@
         <v>39</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>8</v>
@@ -1292,7 +1289,7 @@
         <v>41</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>40</v>
@@ -1330,7 +1327,7 @@
         <v>44</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>42</v>
@@ -1357,7 +1354,7 @@
         <v>46</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" s="4" t="b">
         <v>1</v>
@@ -1370,7 +1367,7 @@
         <v>47</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>45</v>
@@ -1408,7 +1405,7 @@
         <v>49</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>48</v>
@@ -1446,7 +1443,7 @@
         <v>52</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>50</v>
@@ -1484,7 +1481,7 @@
         <v>54</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>53</v>
@@ -1522,7 +1519,7 @@
         <v>57</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>55</v>
@@ -1546,10 +1543,10 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4" t="b">
@@ -1573,7 +1570,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1593,13 +1590,13 @@
         <v>37</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>37</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -1609,7 +1606,7 @@
         <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1629,13 +1626,13 @@
         <v>37</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>37</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -1645,7 +1642,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1665,13 +1662,13 @@
         <v>37</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>37</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
@@ -1696,7 +1693,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>8</v>
@@ -1715,16 +1712,16 @@
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N16" s="5" t="s">
         <v>8</v>
@@ -1734,7 +1731,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>45</v>
@@ -1745,7 +1742,7 @@
         <v>46</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G17" s="5" t="b">
         <v>1</v>
@@ -1755,16 +1752,16 @@
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>45</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N17" s="5" t="s">
         <v>45</v>
@@ -1774,15 +1771,15 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>37</v>
@@ -1793,33 +1790,33 @@
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5" t="b">
@@ -1830,28 +1827,28 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5" t="b">
@@ -1862,20 +1859,20 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1892,26 +1889,26 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1928,26 +1925,26 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1964,16 +1961,16 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
@@ -1998,7 +1995,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>8</v>
@@ -2018,25 +2015,25 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>40</v>
@@ -2056,28 +2053,28 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>40</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -2094,28 +2091,28 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2123,7 +2120,7 @@
         <v>46</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G28" s="4" t="b">
         <v>1</v>
@@ -2134,13 +2131,13 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>45</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>45</v>
@@ -2150,10 +2147,10 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2170,26 +2167,26 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2206,26 +2203,26 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -2242,26 +2239,26 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -2278,26 +2275,26 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -2314,26 +2311,26 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -2350,16 +2347,16 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
@@ -2384,7 +2381,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>8</v>
@@ -2404,28 +2401,28 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>8</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N36" s="5" t="s">
         <v>8</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P36" s="5"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -2442,28 +2439,28 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P37" s="5"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2480,32 +2477,32 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G39" s="5" t="b">
         <v>1</v>
@@ -2516,26 +2513,26 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -2552,16 +2549,16 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
@@ -2594,7 +2591,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2617,27 +2614,27 @@
         <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -2645,16 +2642,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -2673,10 +2670,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -2684,10 +2681,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -2695,10 +2692,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -2730,7 +2727,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2768,26 +2765,26 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2802,9 +2799,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:P1"/>
+      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2894,7 +2891,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2916,13 +2913,13 @@
         <v>39</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>8</v>
@@ -2932,7 +2929,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>40</v>
@@ -2954,13 +2951,13 @@
         <v>41</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>40</v>
@@ -2970,7 +2967,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>42</v>
@@ -2992,13 +2989,13 @@
         <v>44</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>42</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>42</v>
@@ -3008,7 +3005,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>45</v>
@@ -3019,7 +3016,7 @@
         <v>46</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" s="4" t="b">
         <v>1</v>
@@ -3032,13 +3029,13 @@
         <v>47</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>45</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>45</v>
@@ -3183,7 +3180,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -3191,7 +3188,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G11" s="5" t="b">
         <v>1</v>
@@ -3201,19 +3198,19 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>37</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>37</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
@@ -3276,7 +3273,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>8</v>
@@ -3295,16 +3292,16 @@
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>8</v>
@@ -3314,7 +3311,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>45</v>
@@ -3325,7 +3322,7 @@
         <v>46</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G15" s="4" t="b">
         <v>1</v>
@@ -3335,16 +3332,16 @@
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>45</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>45</v>
@@ -3354,7 +3351,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>50</v>
@@ -3373,16 +3370,16 @@
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>50</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>50</v>
@@ -3392,7 +3389,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>42</v>
@@ -3411,16 +3408,16 @@
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>42</v>
@@ -3448,10 +3445,10 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -3459,7 +3456,7 @@
         <v>46</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G19" s="5" t="b">
         <v>1</v>
@@ -3469,29 +3466,29 @@
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -3499,7 +3496,7 @@
         <v>46</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G20" s="5" t="b">
         <v>1</v>
@@ -3509,83 +3506,87 @@
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="H21" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>37</v>
       </c>
       <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="H22" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -3610,7 +3611,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>8</v>
@@ -3629,16 +3630,16 @@
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>8</v>
@@ -3648,10 +3649,10 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3667,29 +3668,29 @@
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -3697,7 +3698,7 @@
         <v>46</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G26" s="4" t="b">
         <v>1</v>
@@ -3707,29 +3708,29 @@
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -3737,7 +3738,7 @@
         <v>46</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>1</v>
@@ -3747,29 +3748,29 @@
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3777,7 +3778,7 @@
         <v>46</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G28" s="4" t="b">
         <v>1</v>
@@ -3787,29 +3788,29 @@
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3825,29 +3826,29 @@
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -3863,115 +3864,121 @@
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
+      <c r="H31" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+      <c r="H32" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+      <c r="H33" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
@@ -3996,10 +4003,10 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -4007,7 +4014,7 @@
         <v>46</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G35" s="5" t="b">
         <v>1</v>
@@ -4017,26 +4024,26 @@
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>45</v>
@@ -4047,7 +4054,7 @@
         <v>46</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G36" s="5" t="b">
         <v>1</v>
@@ -4057,16 +4064,16 @@
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>45</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N36" s="5" t="s">
         <v>45</v>
@@ -4076,10 +4083,10 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -4095,29 +4102,29 @@
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -4133,19 +4140,19 @@
       </c>
       <c r="I38" s="5"/>
       <c r="J38" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
@@ -4170,10 +4177,10 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -4181,7 +4188,7 @@
         <v>46</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G40" s="4" t="b">
         <v>1</v>
@@ -4191,29 +4198,29 @@
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K40" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L40" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="L40" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="M40" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="N40" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="N40" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -4229,51 +4236,53 @@
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
+      <c r="H42" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
@@ -4298,7 +4307,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>8</v>
@@ -4317,16 +4326,16 @@
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>8</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N44" s="5" t="s">
         <v>8</v>
@@ -4336,10 +4345,10 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -4347,7 +4356,7 @@
         <v>46</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G45" s="5" t="b">
         <v>1</v>
@@ -4357,29 +4366,29 @@
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -4395,19 +4404,19 @@
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
@@ -4432,7 +4441,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>8</v>
@@ -4451,16 +4460,16 @@
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>8</v>
@@ -4488,10 +4497,10 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -4507,29 +4516,29 @@
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -4545,19 +4554,19 @@
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
@@ -4582,32 +4591,34 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
+      <c r="H53" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="I53" s="4"/>
       <c r="J53" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O53" s="4"/>
       <c r="P53" s="4"/>
@@ -4632,32 +4643,34 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
+      <c r="H55" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="I55" s="5"/>
       <c r="J55" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
       <c r="M55" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
@@ -4682,10 +4695,10 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -4701,19 +4714,19 @@
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O57" s="4"/>
       <c r="P57" s="4"/>
@@ -4738,10 +4751,10 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -4757,19 +4770,19 @@
       </c>
       <c r="I59" s="5"/>
       <c r="J59" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M59" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O59" s="5"/>
       <c r="P59" s="5"/>
@@ -4794,10 +4807,10 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -4813,19 +4826,19 @@
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O61" s="4"/>
       <c r="P61" s="4"/>
@@ -4850,10 +4863,10 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -4869,19 +4882,19 @@
       </c>
       <c r="I63" s="5"/>
       <c r="J63" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N63" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O63" s="5"/>
       <c r="P63" s="5"/>
@@ -4906,10 +4919,10 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
@@ -4917,7 +4930,7 @@
         <v>46</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G65" s="4" t="b">
         <v>1</v>
@@ -4927,29 +4940,29 @@
       </c>
       <c r="I65" s="4"/>
       <c r="J65" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -4957,7 +4970,7 @@
         <v>46</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G66" s="4" t="b">
         <v>1</v>
@@ -4967,19 +4980,19 @@
       </c>
       <c r="I66" s="4"/>
       <c r="J66" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N66" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O66" s="4"/>
       <c r="P66" s="4"/>
@@ -5011,7 +5024,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -5034,21 +5047,21 @@
         <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -5062,7 +5075,7 @@
         <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -5070,10 +5083,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -5081,13 +5094,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -5095,10 +5108,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -5106,13 +5119,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -5120,13 +5133,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -5134,13 +5147,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -5148,13 +5161,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -5162,10 +5175,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -5173,13 +5186,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -5187,13 +5200,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -5201,13 +5214,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -5215,13 +5228,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -5229,10 +5242,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -5240,10 +5253,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -5251,13 +5264,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -5265,10 +5278,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -5276,13 +5289,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -5290,13 +5303,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>
@@ -5304,13 +5317,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G23" t="b">
         <v>1</v>
@@ -5318,10 +5331,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G24" t="b">
         <v>1</v>
@@ -5329,10 +5342,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G25" t="b">
         <v>1</v>
@@ -5340,10 +5353,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -5351,10 +5364,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
@@ -5362,10 +5375,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G28" t="b">
         <v>1</v>
@@ -5398,7 +5411,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -5428,10 +5441,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -5442,117 +5455,117 @@
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -5587,10 +5600,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" t="s">
         <v>194</v>
-      </c>
-      <c r="B2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5598,7 +5611,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5614,7 +5627,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5622,7 +5635,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5635,7 +5648,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5651,7 +5664,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: typo in Olav rules
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-analytics-olav.xlsx
+++ b/docs/artifacts/rules/dms-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D33C57-3DE0-48D7-B7F1-45DA8EF94421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0318665-649A-4109-B115-1728CFAAFFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="196">
   <si>
     <t>role</t>
   </si>
@@ -255,9 +255,6 @@
   </si>
   <si>
     <t>source</t>
-  </si>
-  <si>
-    <t>geoLoation</t>
   </si>
   <si>
     <t>Point</t>
@@ -1036,10 +1033,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1136,9 +1133,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1251,7 +1248,7 @@
         <v>39</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>8</v>
@@ -1289,7 +1286,7 @@
         <v>41</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>40</v>
@@ -1327,7 +1324,7 @@
         <v>44</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>42</v>
@@ -1354,7 +1351,7 @@
         <v>46</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="4" t="b">
         <v>1</v>
@@ -1367,7 +1364,7 @@
         <v>47</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>45</v>
@@ -1405,7 +1402,7 @@
         <v>49</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>48</v>
@@ -1443,7 +1440,7 @@
         <v>52</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>50</v>
@@ -1481,7 +1478,7 @@
         <v>54</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>53</v>
@@ -1519,7 +1516,7 @@
         <v>57</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>55</v>
@@ -1543,7 +1540,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>59</v>
@@ -1715,7 +1712,7 @@
         <v>64</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>8</v>
@@ -1755,7 +1752,7 @@
         <v>66</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>45</v>
@@ -1779,7 +1776,7 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>37</v>
@@ -1813,7 +1810,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>70</v>
@@ -1845,7 +1842,7 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>70</v>
@@ -2027,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P25" s="4"/>
     </row>
@@ -2065,7 +2062,7 @@
         <v>40</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P26" s="4"/>
     </row>
@@ -2103,7 +2100,7 @@
         <v>75</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P27" s="4"/>
     </row>
@@ -2112,7 +2109,7 @@
         <v>70</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2120,7 +2117,7 @@
         <v>46</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G28" s="4" t="b">
         <v>1</v>
@@ -2150,7 +2147,7 @@
         <v>70</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2170,13 +2167,13 @@
         <v>70</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>70</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
@@ -2186,7 +2183,7 @@
         <v>70</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2206,13 +2203,13 @@
         <v>70</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>70</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
@@ -2222,7 +2219,7 @@
         <v>70</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -2242,13 +2239,13 @@
         <v>70</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M31" s="4" t="s">
         <v>70</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
@@ -2258,7 +2255,7 @@
         <v>70</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -2278,13 +2275,13 @@
         <v>70</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>70</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
@@ -2294,7 +2291,7 @@
         <v>70</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -2314,13 +2311,13 @@
         <v>70</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>70</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
@@ -2330,7 +2327,7 @@
         <v>70</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -2350,13 +2347,13 @@
         <v>70</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>70</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
@@ -2413,7 +2410,7 @@
         <v>8</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P36" s="5"/>
     </row>
@@ -2422,7 +2419,7 @@
         <v>59</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -2442,16 +2439,16 @@
         <v>59</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>59</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P37" s="5"/>
     </row>
@@ -2460,7 +2457,7 @@
         <v>59</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2480,13 +2477,13 @@
         <v>59</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>59</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
@@ -2496,13 +2493,13 @@
         <v>59</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G39" s="5" t="b">
         <v>1</v>
@@ -2516,13 +2513,13 @@
         <v>59</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>59</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
@@ -2532,7 +2529,7 @@
         <v>59</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -2552,13 +2549,13 @@
         <v>59</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>59</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
@@ -2591,7 +2588,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2614,27 +2611,27 @@
         <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -2648,10 +2645,10 @@
         <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -2727,7 +2724,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2799,9 +2796,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
+      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2891,7 +2888,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2913,13 +2910,13 @@
         <v>39</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>8</v>
@@ -2929,7 +2926,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>40</v>
@@ -2951,13 +2948,13 @@
         <v>41</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>40</v>
@@ -2967,7 +2964,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>42</v>
@@ -2989,13 +2986,13 @@
         <v>44</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>42</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>42</v>
@@ -3005,7 +3002,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>45</v>
@@ -3016,7 +3013,7 @@
         <v>46</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="4" t="b">
         <v>1</v>
@@ -3029,13 +3026,13 @@
         <v>47</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>45</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>45</v>
@@ -3180,7 +3177,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -3188,7 +3185,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G11" s="5" t="b">
         <v>1</v>
@@ -3198,19 +3195,19 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>37</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>37</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
@@ -3273,7 +3270,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>8</v>
@@ -3295,13 +3292,13 @@
         <v>64</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>8</v>
@@ -3311,7 +3308,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>45</v>
@@ -3335,13 +3332,13 @@
         <v>66</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>45</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>45</v>
@@ -3351,7 +3348,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>50</v>
@@ -3370,16 +3367,16 @@
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>50</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>50</v>
@@ -3389,7 +3386,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>42</v>
@@ -3408,16 +3405,16 @@
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>42</v>
@@ -3448,7 +3445,7 @@
         <v>63</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -3456,7 +3453,7 @@
         <v>46</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G19" s="5" t="b">
         <v>1</v>
@@ -3466,19 +3463,19 @@
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>63</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>63</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
@@ -3488,7 +3485,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -3496,7 +3493,7 @@
         <v>46</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G20" s="5" t="b">
         <v>1</v>
@@ -3506,19 +3503,19 @@
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>63</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M20" s="5" t="s">
         <v>63</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
@@ -3528,15 +3525,15 @@
         <v>63</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5" t="b">
@@ -3544,7 +3541,7 @@
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -3552,7 +3549,7 @@
         <v>63</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
@@ -3567,7 +3564,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>37</v>
@@ -3611,7 +3608,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>8</v>
@@ -3630,16 +3627,16 @@
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>8</v>
@@ -3649,10 +3646,10 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3668,29 +3665,29 @@
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -3698,7 +3695,7 @@
         <v>46</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G26" s="4" t="b">
         <v>1</v>
@@ -3708,29 +3705,29 @@
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -3738,7 +3735,7 @@
         <v>46</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>1</v>
@@ -3748,29 +3745,29 @@
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3778,7 +3775,7 @@
         <v>46</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G28" s="4" t="b">
         <v>1</v>
@@ -3788,29 +3785,29 @@
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3826,29 +3823,29 @@
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -3864,37 +3861,37 @@
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4" t="b">
@@ -3902,33 +3899,33 @@
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4" t="b">
@@ -3936,33 +3933,33 @@
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4" t="b">
@@ -3970,15 +3967,15 @@
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
@@ -4003,10 +4000,10 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -4014,7 +4011,7 @@
         <v>46</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G35" s="5" t="b">
         <v>1</v>
@@ -4024,26 +4021,26 @@
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>45</v>
@@ -4054,7 +4051,7 @@
         <v>46</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G36" s="5" t="b">
         <v>1</v>
@@ -4064,16 +4061,16 @@
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>45</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N36" s="5" t="s">
         <v>45</v>
@@ -4083,10 +4080,10 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -4102,29 +4099,29 @@
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -4140,19 +4137,19 @@
       </c>
       <c r="I38" s="5"/>
       <c r="J38" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
@@ -4177,10 +4174,10 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -4188,7 +4185,7 @@
         <v>46</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G40" s="4" t="b">
         <v>1</v>
@@ -4198,29 +4195,29 @@
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K40" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="L40" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="L40" s="4" t="s">
-        <v>144</v>
-      </c>
       <c r="M40" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N40" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="N40" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -4236,37 +4233,37 @@
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4" t="b">
@@ -4274,15 +4271,15 @@
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
@@ -4307,7 +4304,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>8</v>
@@ -4326,16 +4323,16 @@
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>8</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N44" s="5" t="s">
         <v>8</v>
@@ -4345,10 +4342,10 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -4356,7 +4353,7 @@
         <v>46</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G45" s="5" t="b">
         <v>1</v>
@@ -4366,29 +4363,29 @@
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -4404,19 +4401,19 @@
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
@@ -4441,7 +4438,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>8</v>
@@ -4460,16 +4457,16 @@
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>8</v>
@@ -4497,10 +4494,10 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -4516,29 +4513,29 @@
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -4554,19 +4551,19 @@
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
@@ -4591,18 +4588,18 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4" t="b">
@@ -4610,15 +4607,15 @@
       </c>
       <c r="I53" s="4"/>
       <c r="J53" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O53" s="4"/>
       <c r="P53" s="4"/>
@@ -4646,15 +4643,15 @@
         <v>65</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G55" s="5"/>
       <c r="H55" s="5" t="b">
@@ -4662,7 +4659,7 @@
       </c>
       <c r="I55" s="5"/>
       <c r="J55" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
@@ -4670,7 +4667,7 @@
         <v>65</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
@@ -4695,10 +4692,10 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -4714,19 +4711,19 @@
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O57" s="4"/>
       <c r="P57" s="4"/>
@@ -4751,10 +4748,10 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -4770,19 +4767,19 @@
       </c>
       <c r="I59" s="5"/>
       <c r="J59" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M59" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O59" s="5"/>
       <c r="P59" s="5"/>
@@ -4807,10 +4804,10 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -4826,19 +4823,19 @@
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O61" s="4"/>
       <c r="P61" s="4"/>
@@ -4863,10 +4860,10 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -4882,19 +4879,19 @@
       </c>
       <c r="I63" s="5"/>
       <c r="J63" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N63" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O63" s="5"/>
       <c r="P63" s="5"/>
@@ -4919,10 +4916,10 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
@@ -4930,7 +4927,7 @@
         <v>46</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G65" s="4" t="b">
         <v>1</v>
@@ -4940,29 +4937,29 @@
       </c>
       <c r="I65" s="4"/>
       <c r="J65" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -4970,7 +4967,7 @@
         <v>46</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G66" s="4" t="b">
         <v>1</v>
@@ -4980,19 +4977,19 @@
       </c>
       <c r="I66" s="4"/>
       <c r="J66" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N66" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O66" s="4"/>
       <c r="P66" s="4"/>
@@ -5024,7 +5021,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -5047,21 +5044,21 @@
         <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -5075,7 +5072,7 @@
         <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -5083,10 +5080,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -5100,7 +5097,7 @@
         <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -5108,10 +5105,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -5119,13 +5116,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -5133,13 +5130,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -5147,13 +5144,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -5161,13 +5158,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -5175,10 +5172,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -5186,13 +5183,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -5200,13 +5197,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -5214,13 +5211,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -5228,13 +5225,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -5242,10 +5239,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -5253,10 +5250,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -5264,13 +5261,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -5278,10 +5275,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -5289,13 +5286,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -5303,13 +5300,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>
@@ -5323,7 +5320,7 @@
         <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" t="b">
         <v>1</v>
@@ -5331,10 +5328,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G24" t="b">
         <v>1</v>
@@ -5342,10 +5339,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G25" t="b">
         <v>1</v>
@@ -5353,10 +5350,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -5364,10 +5361,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
@@ -5375,10 +5372,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G28" t="b">
         <v>1</v>
@@ -5411,7 +5408,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -5441,10 +5438,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -5455,15 +5452,15 @@
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -5474,98 +5471,98 @@
         <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -5600,10 +5597,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" t="s">
         <v>193</v>
-      </c>
-      <c r="B2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5611,7 +5608,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5627,7 +5624,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5635,7 +5632,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5648,7 +5645,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5664,7 +5661,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
refactor: Tutorial examples renaming
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-analytics-olav.xlsx
+++ b/docs/artifacts/rules/dms-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928B0275-2F2D-4299-8A80-6717A50D7781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDC8B24-E5A8-4EF3-857D-3F4E3F1044A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="202">
   <si>
     <t>role</t>
   </si>
@@ -615,6 +615,24 @@
   </si>
   <si>
     <t>edge</t>
+  </si>
+  <si>
+    <t>Class (linage)</t>
+  </si>
+  <si>
+    <t>Property (linage)</t>
+  </si>
+  <si>
+    <t>View Property</t>
+  </si>
+  <si>
+    <t>Connection</t>
+  </si>
+  <si>
+    <t>Is List</t>
+  </si>
+  <si>
+    <t>In Model</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1125,9 +1143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1142,8 +1160,8 @@
     <col min="12" max="12" width="21.44140625" customWidth="1"/>
     <col min="13" max="13" width="14.44140625" customWidth="1"/>
     <col min="14" max="14" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
@@ -1168,10 +1186,10 @@
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>198</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>23</v>
@@ -1180,7 +1198,7 @@
         <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>199</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>26</v>
@@ -1189,7 +1207,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>200</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>29</v>
@@ -1204,16 +1222,16 @@
         <v>32</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>35</v>
+        <v>196</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>36</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -1245,14 +1263,14 @@
       <c r="L3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1283,14 +1301,14 @@
       <c r="L4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1321,14 +1339,14 @@
       <c r="L5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -1361,14 +1379,14 @@
       <c r="L6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -1399,14 +1417,14 @@
       <c r="L7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1437,14 +1455,14 @@
       <c r="L8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -1475,14 +1493,14 @@
       <c r="L9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -1513,14 +1531,14 @@
       <c r="L10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="P10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -1545,14 +1563,14 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="P11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -1581,14 +1599,14 @@
       <c r="L12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="P12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -1617,14 +1635,14 @@
       <c r="L13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="P13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -1653,14 +1671,14 @@
       <c r="L14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="P14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
@@ -1709,14 +1727,14 @@
       <c r="L16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="P16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
@@ -1749,14 +1767,14 @@
       <c r="L17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="P17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
@@ -1783,14 +1801,14 @@
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="5" t="s">
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="P18" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
@@ -1815,14 +1833,14 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="5" t="s">
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="P19" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
@@ -1847,14 +1865,14 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="5" t="s">
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="P20" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
@@ -1883,14 +1901,14 @@
       <c r="L21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="M21" s="5" t="s">
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="P21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
@@ -1919,14 +1937,14 @@
       <c r="L22" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="P22" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
@@ -1955,14 +1973,14 @@
       <c r="L23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="P23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
@@ -2010,15 +2028,15 @@
         <v>8</v>
       </c>
       <c r="M25" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N25" s="4" t="s">
+      <c r="P25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O25" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="P25" s="4"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -2048,15 +2066,15 @@
         <v>40</v>
       </c>
       <c r="M26" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N26" s="4" t="s">
+      <c r="P26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="O26" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
@@ -2086,15 +2104,15 @@
         <v>75</v>
       </c>
       <c r="M27" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N27" s="4" t="s">
+      <c r="P27" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="O27" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="P27" s="4"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
@@ -2125,14 +2143,14 @@
       <c r="L28" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="M28" s="4" t="s">
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N28" s="4" t="s">
+      <c r="P28" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
@@ -2161,14 +2179,14 @@
       <c r="L29" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="M29" s="4" t="s">
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N29" s="4" t="s">
+      <c r="P29" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
@@ -2197,14 +2215,14 @@
       <c r="L30" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M30" s="4" t="s">
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N30" s="4" t="s">
+      <c r="P30" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
@@ -2233,14 +2251,14 @@
       <c r="L31" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="M31" s="4" t="s">
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N31" s="4" t="s">
+      <c r="P31" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
@@ -2269,14 +2287,14 @@
       <c r="L32" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="M32" s="4" t="s">
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N32" s="4" t="s">
+      <c r="P32" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
@@ -2305,14 +2323,14 @@
       <c r="L33" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="M33" s="4" t="s">
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N33" s="4" t="s">
+      <c r="P33" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
@@ -2341,14 +2359,14 @@
       <c r="L34" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="M34" s="4" t="s">
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N34" s="4" t="s">
+      <c r="P34" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
@@ -2396,15 +2414,15 @@
         <v>8</v>
       </c>
       <c r="M36" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="N36" s="5" t="s">
+      <c r="P36" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O36" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="P36" s="5"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
@@ -2434,15 +2452,15 @@
         <v>83</v>
       </c>
       <c r="M37" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="N37" s="5" t="s">
+      <c r="P37" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="O37" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="P37" s="5"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
@@ -2471,14 +2489,14 @@
       <c r="L38" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="M38" s="5" t="s">
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="N38" s="5" t="s">
+      <c r="P38" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
@@ -2507,14 +2525,14 @@
       <c r="L39" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="M39" s="5" t="s">
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="N39" s="5" t="s">
+      <c r="P39" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
@@ -2543,14 +2561,14 @@
       <c r="L40" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="M40" s="5" t="s">
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="N40" s="5" t="s">
+      <c r="P40" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2566,16 +2584,16 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:G4"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13" customWidth="1"/>
+    <col min="2" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
@@ -2591,103 +2609,103 @@
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>201</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>90</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" t="s">
-        <v>76</v>
+      <c r="D3" t="s">
+        <v>187</v>
       </c>
       <c r="E3" t="s">
         <v>187</v>
       </c>
-      <c r="F3" t="s">
-        <v>187</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>65</v>
       </c>
-      <c r="B4" t="s">
-        <v>65</v>
+      <c r="D4" t="s">
+        <v>186</v>
       </c>
       <c r="E4" t="s">
         <v>186</v>
       </c>
-      <c r="F4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>37</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>63</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>63</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>70</v>
       </c>
-      <c r="B7" t="s">
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
         <v>70</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" t="s">
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>59</v>
-      </c>
-      <c r="G8" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2704,14 +2722,14 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="6" width="13" customWidth="1"/>
+    <col min="2" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
@@ -2726,29 +2744,29 @@
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>36</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2756,7 +2774,7 @@
       <c r="A4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2764,7 +2782,7 @@
       <c r="A5" t="s">
         <v>70</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2772,7 +2790,7 @@
       <c r="A6" t="s">
         <v>59</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: updated olav to complete
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-analytics-olav.xlsx
+++ b/docs/artifacts/rules/dms-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C8B8CB-F50D-40A2-873E-C6D9F8FDB97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4498E498-A5BE-45EC-B4BC-41CCD54E4909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="195">
   <si>
     <t>role</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>schema</t>
-  </si>
-  <si>
-    <t>extended</t>
   </si>
   <si>
     <t>extension</t>
@@ -1011,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1033,10 +1030,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1044,30 +1041,27 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1075,29 +1069,32 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
         <v>16</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45388.659870417949</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1105,14 +1102,6 @@
         <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>45388.659870417949</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2">
         <v>45388.659870417949</v>
       </c>
     </row>
@@ -1150,7 +1139,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1170,66 +1159,66 @@
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="O2" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="4" t="b">
         <v>0</v>
@@ -1239,35 +1228,35 @@
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="4" t="b">
         <v>0</v>
@@ -1277,35 +1266,35 @@
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="4" t="b">
         <v>0</v>
@@ -1315,37 +1304,37 @@
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="4" t="b">
         <v>1</v>
@@ -1355,35 +1344,35 @@
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="4" t="b">
         <v>1</v>
@@ -1393,35 +1382,35 @@
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="4" t="b">
         <v>0</v>
@@ -1431,35 +1420,35 @@
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="4" t="b">
         <v>0</v>
@@ -1469,35 +1458,35 @@
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="4" t="b">
         <v>1</v>
@@ -1507,37 +1496,37 @@
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4" t="b">
@@ -1550,24 +1539,24 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="4" t="b">
         <v>1</v>
@@ -1578,32 +1567,32 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="4" t="b">
         <v>1</v>
@@ -1614,32 +1603,32 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="4" t="b">
         <v>1</v>
@@ -1650,18 +1639,18 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -1684,16 +1673,16 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" s="5" t="b">
         <v>0</v>
@@ -1703,37 +1692,37 @@
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" s="5" t="b">
         <v>1</v>
@@ -1743,37 +1732,37 @@
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5" t="b">
@@ -1781,33 +1770,33 @@
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5" t="b">
@@ -1820,26 +1809,26 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5" t="b">
@@ -1852,24 +1841,24 @@
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G21" s="5" t="b">
         <v>1</v>
@@ -1880,32 +1869,32 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" s="5" t="b">
         <v>1</v>
@@ -1916,32 +1905,32 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G23" s="5" t="b">
         <v>1</v>
@@ -1952,18 +1941,18 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
@@ -1986,16 +1975,16 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25" s="4" t="b">
         <v>0</v>
@@ -2006,34 +1995,34 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G26" s="4" t="b">
         <v>0</v>
@@ -2044,34 +2033,34 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>0</v>
@@ -2082,36 +2071,36 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N27" s="4"/>
       <c r="O27" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G28" s="4" t="b">
         <v>1</v>
@@ -2122,32 +2111,32 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G29" s="4" t="b">
         <v>1</v>
@@ -2158,32 +2147,32 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G30" s="4" t="b">
         <v>1</v>
@@ -2194,32 +2183,32 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G31" s="4" t="b">
         <v>1</v>
@@ -2230,32 +2219,32 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G32" s="4" t="b">
         <v>1</v>
@@ -2266,32 +2255,32 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G33" s="4" t="b">
         <v>1</v>
@@ -2302,32 +2291,32 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G34" s="4" t="b">
         <v>1</v>
@@ -2338,18 +2327,18 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P34" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -2372,16 +2361,16 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G36" s="5" t="b">
         <v>0</v>
@@ -2392,34 +2381,34 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G37" s="5" t="b">
         <v>1</v>
@@ -2430,34 +2419,34 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N37" s="5"/>
       <c r="O37" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G38" s="5" t="b">
         <v>1</v>
@@ -2468,32 +2457,32 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G39" s="5" t="b">
         <v>1</v>
@@ -2504,32 +2493,32 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P39" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G40" s="5" t="b">
         <v>0</v>
@@ -2540,18 +2529,18 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P40" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2582,7 +2571,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2593,103 +2582,103 @@
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2718,7 +2707,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2728,54 +2717,54 @@
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2813,7 +2802,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2833,66 +2822,66 @@
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="O2" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="4" t="b">
         <v>0</v>
@@ -2902,35 +2891,35 @@
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="4" t="b">
         <v>0</v>
@@ -2940,35 +2929,35 @@
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="4" t="b">
         <v>0</v>
@@ -2978,37 +2967,37 @@
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="4" t="b">
         <v>1</v>
@@ -3018,21 +3007,21 @@
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -3055,16 +3044,16 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="5" t="b">
         <v>1</v>
@@ -3074,35 +3063,35 @@
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="5" t="b">
         <v>0</v>
@@ -3112,35 +3101,35 @@
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="5" t="b">
         <v>0</v>
@@ -3150,37 +3139,37 @@
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" s="5" t="b">
         <v>1</v>
@@ -3190,35 +3179,35 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="5" t="b">
         <v>1</v>
@@ -3228,21 +3217,21 @@
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -3265,16 +3254,16 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="4" t="b">
         <v>0</v>
@@ -3284,37 +3273,37 @@
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="4" t="b">
         <v>1</v>
@@ -3324,35 +3313,35 @@
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G16" s="4" t="b">
         <v>0</v>
@@ -3362,35 +3351,35 @@
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="4" t="b">
         <v>0</v>
@@ -3400,21 +3389,21 @@
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -3437,18 +3426,18 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G19" s="5" t="b">
         <v>1</v>
@@ -3458,37 +3447,37 @@
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G20" s="5" t="b">
         <v>1</v>
@@ -3498,37 +3487,37 @@
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5" t="b">
@@ -3536,33 +3525,33 @@
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5" t="b">
@@ -3570,17 +3559,17 @@
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
@@ -3603,16 +3592,16 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G24" s="4" t="b">
         <v>0</v>
@@ -3622,35 +3611,35 @@
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25" s="4" t="b">
         <v>1</v>
@@ -3660,37 +3649,37 @@
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" s="4" t="b">
         <v>1</v>
@@ -3700,37 +3689,37 @@
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>1</v>
@@ -3740,37 +3729,37 @@
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G28" s="4" t="b">
         <v>1</v>
@@ -3780,35 +3769,35 @@
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G29" s="4" t="b">
         <v>0</v>
@@ -3818,35 +3807,35 @@
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G30" s="4" t="b">
         <v>0</v>
@@ -3856,37 +3845,37 @@
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4" t="b">
@@ -3894,33 +3883,33 @@
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4" t="b">
@@ -3928,33 +3917,33 @@
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4" t="b">
@@ -3962,17 +3951,17 @@
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
@@ -3995,18 +3984,18 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G35" s="5" t="b">
         <v>1</v>
@@ -4016,37 +4005,37 @@
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P35" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G36" s="5" t="b">
         <v>1</v>
@@ -4056,35 +4045,35 @@
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G37" s="5" t="b">
         <v>0</v>
@@ -4094,35 +4083,35 @@
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G38" s="5" t="b">
         <v>1</v>
@@ -4132,21 +4121,21 @@
       </c>
       <c r="I38" s="5"/>
       <c r="J38" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
@@ -4169,18 +4158,18 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G40" s="4" t="b">
         <v>1</v>
@@ -4190,35 +4179,35 @@
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K40" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L40" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="P40" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="P40" s="4" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G41" s="4" t="b">
         <v>0</v>
@@ -4228,37 +4217,37 @@
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P41" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4" t="b">
@@ -4266,17 +4255,17 @@
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P42" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -4299,16 +4288,16 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G44" s="5" t="b">
         <v>0</v>
@@ -4318,37 +4307,37 @@
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P44" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G45" s="5" t="b">
         <v>1</v>
@@ -4358,35 +4347,35 @@
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P45" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G46" s="5" t="b">
         <v>0</v>
@@ -4396,21 +4385,21 @@
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P46" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -4433,16 +4422,16 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G48" s="4" t="b">
         <v>0</v>
@@ -4452,21 +4441,21 @@
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P48" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
@@ -4489,16 +4478,16 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G50" s="5" t="b">
         <v>0</v>
@@ -4508,35 +4497,35 @@
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P50" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G51" s="5" t="b">
         <v>0</v>
@@ -4546,21 +4535,21 @@
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P51" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
@@ -4583,18 +4572,18 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4" t="b">
@@ -4602,17 +4591,17 @@
       </c>
       <c r="I53" s="4"/>
       <c r="J53" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P53" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
@@ -4635,18 +4624,18 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G55" s="5"/>
       <c r="H55" s="5" t="b">
@@ -4654,17 +4643,17 @@
       </c>
       <c r="I55" s="5"/>
       <c r="J55" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>
       <c r="N55" s="5"/>
       <c r="O55" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P55" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
@@ -4687,16 +4676,16 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G57" s="4" t="b">
         <v>1</v>
@@ -4706,21 +4695,21 @@
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P57" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
@@ -4743,16 +4732,16 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G59" s="5" t="b">
         <v>1</v>
@@ -4762,21 +4751,21 @@
       </c>
       <c r="I59" s="5"/>
       <c r="J59" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M59" s="5"/>
       <c r="N59" s="5"/>
       <c r="O59" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P59" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
@@ -4799,16 +4788,16 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G61" s="4" t="b">
         <v>1</v>
@@ -4818,21 +4807,21 @@
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P61" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
@@ -4855,16 +4844,16 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G63" s="5" t="b">
         <v>0</v>
@@ -4874,21 +4863,21 @@
       </c>
       <c r="I63" s="5"/>
       <c r="J63" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
       <c r="O63" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P63" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.3">
@@ -4911,18 +4900,18 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G65" s="4" t="b">
         <v>1</v>
@@ -4932,37 +4921,37 @@
       </c>
       <c r="I65" s="4"/>
       <c r="J65" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
       <c r="O65" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P65" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G66" s="4" t="b">
         <v>1</v>
@@ -4972,21 +4961,21 @@
       </c>
       <c r="I66" s="4"/>
       <c r="J66" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
       <c r="O66" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P66" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -5017,7 +5006,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -5028,353 +5017,353 @@
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F26" t="b">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -5403,7 +5392,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -5413,151 +5402,151 @@
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -5572,8 +5561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5592,10 +5581,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" t="s">
         <v>185</v>
-      </c>
-      <c r="B2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5603,65 +5592,65 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2">
         <v>45388.659870442891</v>
@@ -5669,7 +5658,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2">
         <v>45388.659870442891</v>
@@ -5677,10 +5666,10 @@
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[NEAT-237, NEAT-262] 🫠Adding Svein Harald Spreadsheets (#459)
* tests: clearer names

* fix: bug in DMSToRules step

* fix: DMSImporter download enterprise model

* fix; conversion dms to info

* fix: added missing conversion

* fix: logic bug

* refactor: Added Svein Harald spredsheet

* fix: Include metadata sheet

* tests: extending excel importer to svein harald

* fix: bug in ExcelImporter

* refactor: first pass at refactoring DMS validation

* refactor: update validation

* refactor: updated olav to complete

* refactor: update validation

* refactor: update rules

* tests: updated failing test

* docs: Added Svein Harald DMS rules

* tests: Added Svein Harald to tests

* fix: Bug in DMS serializer

* tests: failing tests

* tests: for bad conversion

* fix: missing parent in InfoInput rules

* refactor; fix svein harald

* refactor; revert changes

* refactor: review feedback
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-analytics-olav.xlsx
+++ b/docs/artifacts/rules/dms-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C8B8CB-F50D-40A2-873E-C6D9F8FDB97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4498E498-A5BE-45EC-B4BC-41CCD54E4909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="195">
   <si>
     <t>role</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>schema</t>
-  </si>
-  <si>
-    <t>extended</t>
   </si>
   <si>
     <t>extension</t>
@@ -1011,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1033,10 +1030,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1044,30 +1041,27 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1075,29 +1069,32 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
         <v>16</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45388.659870417949</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1105,14 +1102,6 @@
         <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>45388.659870417949</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2">
         <v>45388.659870417949</v>
       </c>
     </row>
@@ -1150,7 +1139,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1170,66 +1159,66 @@
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="O2" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="4" t="b">
         <v>0</v>
@@ -1239,35 +1228,35 @@
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="4" t="b">
         <v>0</v>
@@ -1277,35 +1266,35 @@
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="4" t="b">
         <v>0</v>
@@ -1315,37 +1304,37 @@
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="4" t="b">
         <v>1</v>
@@ -1355,35 +1344,35 @@
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="4" t="b">
         <v>1</v>
@@ -1393,35 +1382,35 @@
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="4" t="b">
         <v>0</v>
@@ -1431,35 +1420,35 @@
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="4" t="b">
         <v>0</v>
@@ -1469,35 +1458,35 @@
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="4" t="b">
         <v>1</v>
@@ -1507,37 +1496,37 @@
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4" t="b">
@@ -1550,24 +1539,24 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="4" t="b">
         <v>1</v>
@@ -1578,32 +1567,32 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="4" t="b">
         <v>1</v>
@@ -1614,32 +1603,32 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="4" t="b">
         <v>1</v>
@@ -1650,18 +1639,18 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -1684,16 +1673,16 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" s="5" t="b">
         <v>0</v>
@@ -1703,37 +1692,37 @@
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" s="5" t="b">
         <v>1</v>
@@ -1743,37 +1732,37 @@
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5" t="b">
@@ -1781,33 +1770,33 @@
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5" t="b">
@@ -1820,26 +1809,26 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5" t="b">
@@ -1852,24 +1841,24 @@
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G21" s="5" t="b">
         <v>1</v>
@@ -1880,32 +1869,32 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" s="5" t="b">
         <v>1</v>
@@ -1916,32 +1905,32 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G23" s="5" t="b">
         <v>1</v>
@@ -1952,18 +1941,18 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
@@ -1986,16 +1975,16 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25" s="4" t="b">
         <v>0</v>
@@ -2006,34 +1995,34 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G26" s="4" t="b">
         <v>0</v>
@@ -2044,34 +2033,34 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>0</v>
@@ -2082,36 +2071,36 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N27" s="4"/>
       <c r="O27" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G28" s="4" t="b">
         <v>1</v>
@@ -2122,32 +2111,32 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G29" s="4" t="b">
         <v>1</v>
@@ -2158,32 +2147,32 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G30" s="4" t="b">
         <v>1</v>
@@ -2194,32 +2183,32 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G31" s="4" t="b">
         <v>1</v>
@@ -2230,32 +2219,32 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G32" s="4" t="b">
         <v>1</v>
@@ -2266,32 +2255,32 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G33" s="4" t="b">
         <v>1</v>
@@ -2302,32 +2291,32 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G34" s="4" t="b">
         <v>1</v>
@@ -2338,18 +2327,18 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P34" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -2372,16 +2361,16 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G36" s="5" t="b">
         <v>0</v>
@@ -2392,34 +2381,34 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G37" s="5" t="b">
         <v>1</v>
@@ -2430,34 +2419,34 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N37" s="5"/>
       <c r="O37" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G38" s="5" t="b">
         <v>1</v>
@@ -2468,32 +2457,32 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G39" s="5" t="b">
         <v>1</v>
@@ -2504,32 +2493,32 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P39" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G40" s="5" t="b">
         <v>0</v>
@@ -2540,18 +2529,18 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P40" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2582,7 +2571,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2593,103 +2582,103 @@
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2718,7 +2707,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2728,54 +2717,54 @@
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2813,7 +2802,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2833,66 +2822,66 @@
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="O2" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="4" t="b">
         <v>0</v>
@@ -2902,35 +2891,35 @@
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="4" t="b">
         <v>0</v>
@@ -2940,35 +2929,35 @@
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="4" t="b">
         <v>0</v>
@@ -2978,37 +2967,37 @@
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="4" t="b">
         <v>1</v>
@@ -3018,21 +3007,21 @@
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -3055,16 +3044,16 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="5" t="b">
         <v>1</v>
@@ -3074,35 +3063,35 @@
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="5" t="b">
         <v>0</v>
@@ -3112,35 +3101,35 @@
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="5" t="b">
         <v>0</v>
@@ -3150,37 +3139,37 @@
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" s="5" t="b">
         <v>1</v>
@@ -3190,35 +3179,35 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="5" t="b">
         <v>1</v>
@@ -3228,21 +3217,21 @@
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -3265,16 +3254,16 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="4" t="b">
         <v>0</v>
@@ -3284,37 +3273,37 @@
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="4" t="b">
         <v>1</v>
@@ -3324,35 +3313,35 @@
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G16" s="4" t="b">
         <v>0</v>
@@ -3362,35 +3351,35 @@
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="4" t="b">
         <v>0</v>
@@ -3400,21 +3389,21 @@
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -3437,18 +3426,18 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G19" s="5" t="b">
         <v>1</v>
@@ -3458,37 +3447,37 @@
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G20" s="5" t="b">
         <v>1</v>
@@ -3498,37 +3487,37 @@
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5" t="b">
@@ -3536,33 +3525,33 @@
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5" t="b">
@@ -3570,17 +3559,17 @@
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
@@ -3603,16 +3592,16 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G24" s="4" t="b">
         <v>0</v>
@@ -3622,35 +3611,35 @@
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25" s="4" t="b">
         <v>1</v>
@@ -3660,37 +3649,37 @@
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" s="4" t="b">
         <v>1</v>
@@ -3700,37 +3689,37 @@
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>1</v>
@@ -3740,37 +3729,37 @@
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G28" s="4" t="b">
         <v>1</v>
@@ -3780,35 +3769,35 @@
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G29" s="4" t="b">
         <v>0</v>
@@ -3818,35 +3807,35 @@
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G30" s="4" t="b">
         <v>0</v>
@@ -3856,37 +3845,37 @@
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4" t="b">
@@ -3894,33 +3883,33 @@
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4" t="b">
@@ -3928,33 +3917,33 @@
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4" t="b">
@@ -3962,17 +3951,17 @@
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
@@ -3995,18 +3984,18 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G35" s="5" t="b">
         <v>1</v>
@@ -4016,37 +4005,37 @@
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P35" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G36" s="5" t="b">
         <v>1</v>
@@ -4056,35 +4045,35 @@
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G37" s="5" t="b">
         <v>0</v>
@@ -4094,35 +4083,35 @@
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G38" s="5" t="b">
         <v>1</v>
@@ -4132,21 +4121,21 @@
       </c>
       <c r="I38" s="5"/>
       <c r="J38" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
@@ -4169,18 +4158,18 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G40" s="4" t="b">
         <v>1</v>
@@ -4190,35 +4179,35 @@
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K40" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L40" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="P40" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="P40" s="4" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G41" s="4" t="b">
         <v>0</v>
@@ -4228,37 +4217,37 @@
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P41" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4" t="b">
@@ -4266,17 +4255,17 @@
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P42" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -4299,16 +4288,16 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G44" s="5" t="b">
         <v>0</v>
@@ -4318,37 +4307,37 @@
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P44" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G45" s="5" t="b">
         <v>1</v>
@@ -4358,35 +4347,35 @@
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P45" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G46" s="5" t="b">
         <v>0</v>
@@ -4396,21 +4385,21 @@
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P46" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -4433,16 +4422,16 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G48" s="4" t="b">
         <v>0</v>
@@ -4452,21 +4441,21 @@
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P48" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
@@ -4489,16 +4478,16 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G50" s="5" t="b">
         <v>0</v>
@@ -4508,35 +4497,35 @@
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P50" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G51" s="5" t="b">
         <v>0</v>
@@ -4546,21 +4535,21 @@
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P51" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
@@ -4583,18 +4572,18 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4" t="b">
@@ -4602,17 +4591,17 @@
       </c>
       <c r="I53" s="4"/>
       <c r="J53" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P53" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
@@ -4635,18 +4624,18 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G55" s="5"/>
       <c r="H55" s="5" t="b">
@@ -4654,17 +4643,17 @@
       </c>
       <c r="I55" s="5"/>
       <c r="J55" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>
       <c r="N55" s="5"/>
       <c r="O55" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P55" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
@@ -4687,16 +4676,16 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G57" s="4" t="b">
         <v>1</v>
@@ -4706,21 +4695,21 @@
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P57" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
@@ -4743,16 +4732,16 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G59" s="5" t="b">
         <v>1</v>
@@ -4762,21 +4751,21 @@
       </c>
       <c r="I59" s="5"/>
       <c r="J59" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M59" s="5"/>
       <c r="N59" s="5"/>
       <c r="O59" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P59" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
@@ -4799,16 +4788,16 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G61" s="4" t="b">
         <v>1</v>
@@ -4818,21 +4807,21 @@
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P61" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
@@ -4855,16 +4844,16 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G63" s="5" t="b">
         <v>0</v>
@@ -4874,21 +4863,21 @@
       </c>
       <c r="I63" s="5"/>
       <c r="J63" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
       <c r="O63" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P63" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.3">
@@ -4911,18 +4900,18 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G65" s="4" t="b">
         <v>1</v>
@@ -4932,37 +4921,37 @@
       </c>
       <c r="I65" s="4"/>
       <c r="J65" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
       <c r="O65" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P65" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G66" s="4" t="b">
         <v>1</v>
@@ -4972,21 +4961,21 @@
       </c>
       <c r="I66" s="4"/>
       <c r="J66" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
       <c r="O66" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P66" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -5017,7 +5006,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -5028,353 +5017,353 @@
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F26" t="b">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -5403,7 +5392,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -5413,151 +5402,151 @@
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -5572,8 +5561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5592,10 +5581,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" t="s">
         <v>185</v>
-      </c>
-      <c r="B2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5603,65 +5592,65 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2">
         <v>45388.659870442891</v>
@@ -5669,7 +5658,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2">
         <v>45388.659870442891</v>
@@ -5677,10 +5666,10 @@
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: update tutorial artifact
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-analytics-olav.xlsx
+++ b/docs/artifacts/rules/dms-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C020C0A-C1E8-418F-A510-A9E73D545B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCC0CA8-D6AB-40A2-B305-972175D262C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -617,7 +617,7 @@
     <t>Immutable</t>
   </si>
   <si>
-    <t>WindTurbine(type=power:WindFarm.windTurbines)</t>
+    <t>edge(type=power:WindFarm.windTurbines)</t>
   </si>
 </sst>
 </file>
@@ -1120,9 +1120,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,7 +1131,7 @@
     <col min="2" max="2" width="21.44140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="5" max="5" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.77734375" customWidth="1"/>
     <col min="7" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="42.44140625" customWidth="1"/>
@@ -1810,10 +1810,10 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>196</v>
+        <v>30</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -2889,16 +2889,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.44140625" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="5" width="13" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="53.44140625" customWidth="1"/>
@@ -3711,10 +3712,10 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>196</v>
+        <v>30</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>

</xml_diff>